<commit_message>
add quelimane health facilities
</commit_message>
<xml_diff>
--- a/mentoring-core/health-facility-mapping.xlsx
+++ b/mentoring-core/health-facility-mapping.xlsx
@@ -13,13 +13,14 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$2:$E$116</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$B$2:$E$116</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$B$2:$E$116</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="151">
   <si>
     <t>Province</t>
   </si>
@@ -418,6 +419,60 @@
   </si>
   <si>
     <t>CS Txalalane</t>
+  </si>
+  <si>
+    <t>Quelimane</t>
+  </si>
+  <si>
+    <t>CS 17 de Setembro</t>
+  </si>
+  <si>
+    <t>CS 24 de Julho</t>
+  </si>
+  <si>
+    <t>CS 4 de Dezembro</t>
+  </si>
+  <si>
+    <t>CS Chabeco</t>
+  </si>
+  <si>
+    <t>CS Coalane</t>
+  </si>
+  <si>
+    <t>CS Incidua</t>
+  </si>
+  <si>
+    <t>CS Inhangulue</t>
+  </si>
+  <si>
+    <t>CS Malanha</t>
+  </si>
+  <si>
+    <t>CS Maquival Rio</t>
+  </si>
+  <si>
+    <t>CS Maquival Sede</t>
+  </si>
+  <si>
+    <t>CS Micajune</t>
+  </si>
+  <si>
+    <t>CS Namuinho</t>
+  </si>
+  <si>
+    <t>CS Penitenciário</t>
+  </si>
+  <si>
+    <t>CS Sagariveira</t>
+  </si>
+  <si>
+    <t>CS Varela</t>
+  </si>
+  <si>
+    <t>CS Zalala</t>
+  </si>
+  <si>
+    <t>HG Quelimane</t>
   </si>
 </sst>
 </file>
@@ -427,7 +482,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -455,6 +510,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -499,13 +559,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -529,10 +593,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E116"/>
+  <dimension ref="B2:E134"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A87" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E115" activeCellId="0" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2155,6 +2219,258 @@
         <v>132</v>
       </c>
     </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B118" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B119" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B120" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B121" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E123" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B124" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B125" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B126" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B127" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E127" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B128" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E128" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C131" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E131" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E132" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C133" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E133" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C134" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E134" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="B2:E116"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>